<commit_message>
Update detection field test data.xlsx
</commit_message>
<xml_diff>
--- a/detection field test data.xlsx
+++ b/detection field test data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shosh\OneDrive\2 PhD\Projects\Detection dog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f3a69dc1a79d235a/2 PhD/GIT/detection-dog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84068825-A51A-45D9-9695-B1875DA6DCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{84068825-A51A-45D9-9695-B1875DA6DCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AB7BA88-4566-4569-B4FA-6835DAA20DAD}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2865" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{78F3DDC6-AADC-4A30-A654-FCA5E2B59584}"/>
+    <workbookView xWindow="28680" yWindow="-2865" windowWidth="29040" windowHeight="15720" xr2:uid="{78F3DDC6-AADC-4A30-A654-FCA5E2B59584}"/>
   </bookViews>
   <sheets>
     <sheet name="dog" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -109,13 +109,19 @@
   </si>
   <si>
     <t>42 minutes 48 seconds</t>
+  </si>
+  <si>
+    <t>14 minutes 27 seconds</t>
+  </si>
+  <si>
+    <t>Worked uphill. Picked up odour pooling around trees uphill of target and then worked back down to target. Koda slightly hot.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,27 +496,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35957C9B-8F96-413D-BC7D-E3550DA63DD4}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.08203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="146" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -540,7 +545,7 @@
       <c r="I1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -550,9 +555,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>45752</v>
+        <v>45766</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
@@ -578,7 +583,7 @@
       <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2">
         <v>594</v>
       </c>
       <c r="K2" s="2" t="s">
@@ -588,9 +593,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>45753</v>
+        <v>45767</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
@@ -616,7 +621,7 @@
       <c r="I3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3">
         <v>451</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -624,6 +629,44 @@
       </c>
       <c r="L3" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>45772</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E4">
+        <v>23</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4">
+        <v>867</v>
+      </c>
+      <c r="K4" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -635,21 +678,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A64F118-EA99-4C9D-A343-CF56CB35EAE1}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.08203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -675,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>45753</v>
       </c>
@@ -691,7 +734,7 @@
       <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2">
         <v>2568</v>
       </c>
       <c r="G2" t="s">
@@ -701,100 +744,100 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="6:6">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="6:6">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="6:6">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="6:6">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="6:6">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="6:6">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="6:6">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="6:6">
+    <row r="26" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="6:6">
+    <row r="27" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="6:6">
+    <row r="28" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="6:6">
+    <row r="29" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="6:6">
+    <row r="30" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="6:6">
+    <row r="31" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="6:6">
+    <row r="32" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="6:6">
+    <row r="33" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F33" s="2"/>
     </row>
-    <row r="34" spans="6:6">
+    <row r="34" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F34" s="2"/>
     </row>
   </sheetData>

</xml_diff>